<commit_message>
Combine Florenceville and Bristol prior to 2009
Starting with 2009, Florenceville and Bristol were amalgamated into Florenceville-Bristol. For data consistency, we manually combine the two in the 2000 through to 2008 'data_final' data (with 'data_clean' serving as a record of the pre-manipulation data), weighting fields like Average Tax Rate as appropriate.
</commit_message>
<xml_diff>
--- a/data/data_final/data_pol_prov.xlsx
+++ b/data/data_final/data_pol_prov.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
   <si>
     <t>Municipality</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Bouctouche</t>
   </si>
   <si>
-    <t>Bristol</t>
-  </si>
-  <si>
     <t>Cambridge-Narrows</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
   </si>
   <si>
     <t>Eel River Crossing</t>
-  </si>
-  <si>
-    <t>Florenceville</t>
   </si>
   <si>
     <t>Florenceville-Bristol</t>
@@ -402,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B105" totalsRowShown="0">
-  <autoFilter ref="A1:B105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B103" totalsRowShown="0">
+  <autoFilter ref="A1:B103"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Municipality" dataDxfId="0"/>
     <tableColumn id="2" name="Policing Provider" dataDxfId="0"/>
@@ -697,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -840,7 +834,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -848,7 +842,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -912,7 +906,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -920,7 +914,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -928,7 +922,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -936,7 +930,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -952,7 +946,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -968,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -984,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1000,7 +994,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1016,7 +1010,7 @@
         <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1024,7 +1018,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1040,7 +1034,7 @@
         <v>45</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1136,7 +1130,7 @@
         <v>57</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1144,7 +1138,7 @@
         <v>58</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1152,7 +1146,7 @@
         <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1160,7 +1154,7 @@
         <v>60</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1168,7 +1162,7 @@
         <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1184,7 +1178,7 @@
         <v>63</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1192,7 +1186,7 @@
         <v>64</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1208,7 +1202,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1216,7 +1210,7 @@
         <v>67</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1232,7 +1226,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1240,7 +1234,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1272,7 +1266,7 @@
         <v>74</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1288,7 +1282,7 @@
         <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1296,7 +1290,7 @@
         <v>77</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1304,7 +1298,7 @@
         <v>78</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1320,7 +1314,7 @@
         <v>80</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1328,7 +1322,7 @@
         <v>81</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1336,7 +1330,7 @@
         <v>82</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1344,7 +1338,7 @@
         <v>83</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1352,7 +1346,7 @@
         <v>84</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1360,7 +1354,7 @@
         <v>85</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1368,7 +1362,7 @@
         <v>86</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1504,7 +1498,7 @@
         <v>103</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1520,7 +1514,7 @@
         <v>105</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1528,22 +1522,6 @@
         <v>106</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B105" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combine Florenceville and Bristol prior to 2009 (#4)
Starting with 2009, Florenceville and Bristol were amalgamated into Florenceville-Bristol. For data consistency, we manually combine the two in the 2000 through to 2008 'data_final' data (with 'data_clean' serving as a record of the pre-manipulation data), weighting fields like Average Tax Rate as appropriate.
</commit_message>
<xml_diff>
--- a/data/data_final/data_pol_prov.xlsx
+++ b/data/data_final/data_pol_prov.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
   <si>
     <t>Municipality</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Bouctouche</t>
   </si>
   <si>
-    <t>Bristol</t>
-  </si>
-  <si>
     <t>Cambridge-Narrows</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
   </si>
   <si>
     <t>Eel River Crossing</t>
-  </si>
-  <si>
-    <t>Florenceville</t>
   </si>
   <si>
     <t>Florenceville-Bristol</t>
@@ -402,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B105" totalsRowShown="0">
-  <autoFilter ref="A1:B105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B103" totalsRowShown="0">
+  <autoFilter ref="A1:B103"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Municipality" dataDxfId="0"/>
     <tableColumn id="2" name="Policing Provider" dataDxfId="0"/>
@@ -697,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -840,7 +834,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -848,7 +842,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -912,7 +906,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -920,7 +914,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -928,7 +922,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -936,7 +930,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -952,7 +946,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -968,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -984,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1000,7 +994,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1016,7 +1010,7 @@
         <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1024,7 +1018,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1040,7 +1034,7 @@
         <v>45</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1136,7 +1130,7 @@
         <v>57</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1144,7 +1138,7 @@
         <v>58</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1152,7 +1146,7 @@
         <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1160,7 +1154,7 @@
         <v>60</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1168,7 +1162,7 @@
         <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1184,7 +1178,7 @@
         <v>63</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1192,7 +1186,7 @@
         <v>64</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1208,7 +1202,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1216,7 +1210,7 @@
         <v>67</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1232,7 +1226,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1240,7 +1234,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1272,7 +1266,7 @@
         <v>74</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1288,7 +1282,7 @@
         <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1296,7 +1290,7 @@
         <v>77</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1304,7 +1298,7 @@
         <v>78</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1320,7 +1314,7 @@
         <v>80</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1328,7 +1322,7 @@
         <v>81</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1336,7 +1330,7 @@
         <v>82</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1344,7 +1338,7 @@
         <v>83</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1352,7 +1346,7 @@
         <v>84</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1360,7 +1354,7 @@
         <v>85</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1368,7 +1362,7 @@
         <v>86</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1504,7 +1498,7 @@
         <v>103</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1520,7 +1514,7 @@
         <v>105</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1528,22 +1522,6 @@
         <v>106</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B105" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>